<commit_message>
change Dialog to List and Grid
</commit_message>
<xml_diff>
--- a/public/feed.xlsx
+++ b/public/feed.xlsx
@@ -170,10 +170,10 @@
     <t>{label: "Новый текст ", editable: 1}</t>
   </si>
   <si>
-    <t>{ label: "Текст вверху", editable: 1}</t>
-  </si>
-  <si>
-    <t>{label: "Текст внизу", editable: 1}</t>
+    <t>{label: "Текст внизу", editable: 2}</t>
+  </si>
+  <si>
+    <t>{ label: "Текст  вверху", editable: "yes"}</t>
   </si>
 </sst>
 </file>
@@ -787,7 +787,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.53515625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -810,13 +810,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>43</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="5" customFormat="1" ht="12.45" x14ac:dyDescent="0.3">

</xml_diff>